<commit_message>
- updated express js
</commit_message>
<xml_diff>
--- a/All in One/excel/HTML CSS JS.xlsx
+++ b/All in One/excel/HTML CSS JS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="8265" tabRatio="656" firstSheet="4" activeTab="9"/>
+    <workbookView windowWidth="18600" windowHeight="6800" tabRatio="656" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="cmd propmpt" sheetId="11" r:id="rId1"/>
@@ -9866,6 +9866,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Node Package Manager (NPM) provides two main functionalities</t>
     </r>
     <r>
@@ -9893,6 +9901,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Check NPM Version</t>
     </r>
     <r>
@@ -9944,6 +9960,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Install Modules</t>
     </r>
     <r>
@@ -10122,6 +10146,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">install Modules using NPM </t>
     </r>
     <r>
@@ -10225,6 +10257,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>check installed Modules</t>
     </r>
     <r>
@@ -10330,6 +10370,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Uninstall Modules</t>
     </r>
     <r>
@@ -10417,6 +10465,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Custom Modules</t>
     </r>
     <r>
@@ -10594,6 +10650,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>package.json</t>
     </r>
     <r>
@@ -10633,6 +10697,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>package-lock.json</t>
     </r>
     <r>
@@ -10671,6 +10743,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>node module</t>
     </r>
     <r>
@@ -10709,6 +10789,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">2. Command line utility to install Node.js packages, do version management and dependency management of Node.js packages.
 </t>
     </r>
@@ -10737,6 +10824,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Update NPM Version</t>
     </r>
     <r>
@@ -10926,6 +11021,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">install Modules locally using NPM </t>
     </r>
     <r>
@@ -11092,6 +11195,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Update NPM</t>
     </r>
     <r>
@@ -11311,6 +11422,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Search Modules</t>
     </r>
     <r>
@@ -11398,6 +11517,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Update Modules</t>
     </r>
     <r>
@@ -11491,6 +11618,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Don't push node_modules on git
 becaues it is a very big file . because it contains all packages
 </t>
@@ -17820,10 +17954,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="102">
     <font>
@@ -18121,6 +18255,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -18130,7 +18279,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18138,31 +18287,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18189,17 +18316,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18214,6 +18340,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -18221,16 +18355,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18250,8 +18383,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -18626,7 +18760,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18638,49 +18778,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18692,13 +18844,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18710,73 +18862,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18794,7 +18880,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18806,7 +18922,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -18883,28 +19017,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -18926,24 +19049,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -18959,6 +19078,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -18985,106 +19119,136 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="55" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -19093,40 +19257,10 @@
     <xf numFmtId="0" fontId="45" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -19838,20 +19972,20 @@
       <selection pane="topRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="27.5714285714286" style="42" customWidth="1"/>
-    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="27.5727272727273" style="42" customWidth="1"/>
+    <col min="2" max="2" width="13.2818181818182" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="28.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="32.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="52.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="45.1428571428571" customWidth="1"/>
-    <col min="8" max="8" width="66.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="82.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="28.4272727272727" customWidth="1"/>
+    <col min="5" max="5" width="32.8545454545455" customWidth="1"/>
+    <col min="6" max="6" width="52.7181818181818" customWidth="1"/>
+    <col min="7" max="7" width="45.1454545454545" customWidth="1"/>
+    <col min="8" max="8" width="66.1454545454545" customWidth="1"/>
+    <col min="10" max="10" width="82.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15.75" spans="1:10">
+    <row r="3" ht="17" spans="1:10">
       <c r="A3" s="43" t="s">
         <v>0</v>
       </c>
@@ -19877,7 +20011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="28.5" spans="1:10">
+    <row r="4" ht="27" spans="1:10">
       <c r="A4" s="43"/>
       <c r="C4" s="4"/>
       <c r="D4" s="112" t="s">
@@ -19897,7 +20031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" ht="42.75" spans="1:10">
+    <row r="5" ht="40.5" spans="1:10">
       <c r="A5" s="43"/>
       <c r="C5" s="4"/>
       <c r="D5" s="108" t="s">
@@ -19917,7 +20051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="31.5" spans="1:10">
+    <row r="6" ht="34" spans="1:10">
       <c r="A6" s="43"/>
       <c r="C6" s="4"/>
       <c r="D6" s="112" t="s">
@@ -19937,7 +20071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="28.5" spans="1:10">
+    <row r="7" ht="27" spans="1:10">
       <c r="A7" s="43"/>
       <c r="C7" s="4"/>
       <c r="D7" s="112" t="s">
@@ -19957,7 +20091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" ht="28.5" spans="1:10">
+    <row r="8" ht="27" spans="1:10">
       <c r="A8" s="43"/>
       <c r="C8" s="10" t="s">
         <v>24</v>
@@ -19979,7 +20113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" ht="28.5" spans="1:10">
+    <row r="9" ht="17" spans="1:10">
       <c r="A9" s="43"/>
       <c r="C9" s="10"/>
       <c r="D9" s="115" t="s">
@@ -19999,7 +20133,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" ht="42.75" spans="1:10">
+    <row r="10" ht="40.5" spans="1:10">
       <c r="A10" s="43"/>
       <c r="C10" s="10"/>
       <c r="D10" s="117" t="s">
@@ -20121,7 +20255,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="1018" ht="30" spans="1:8">
+    <row r="1018" ht="29" spans="1:8">
       <c r="A1018" s="122"/>
       <c r="H1018" s="4" t="s">
         <v>55</v>
@@ -20193,7 +20327,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1030" s="4" customFormat="1" ht="30" spans="1:8">
+    <row r="1030" s="4" customFormat="1" ht="29" spans="1:8">
       <c r="A1030" s="60"/>
       <c r="H1030" s="4" t="s">
         <v>67</v>
@@ -20229,7 +20363,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="1036" s="4" customFormat="1" ht="30" spans="1:8">
+    <row r="1036" s="4" customFormat="1" spans="1:8">
       <c r="A1036" s="60"/>
       <c r="H1036" s="4" t="s">
         <v>73</v>
@@ -20588,28 +20722,28 @@
   <sheetPr/>
   <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="29.5714285714286" style="42" customWidth="1"/>
-    <col min="3" max="3" width="43.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="50.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="29.5727272727273" style="42" customWidth="1"/>
+    <col min="3" max="3" width="43.7181818181818" customWidth="1"/>
+    <col min="4" max="4" width="50.1454545454545" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
-    <col min="6" max="6" width="51.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="52.5714285714286" customWidth="1"/>
-    <col min="8" max="8" width="54.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="52.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="26.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="51.2818181818182" customWidth="1"/>
+    <col min="7" max="7" width="52.5727272727273" customWidth="1"/>
+    <col min="8" max="8" width="54.8545454545455" customWidth="1"/>
+    <col min="9" max="9" width="52.1454545454545" customWidth="1"/>
+    <col min="10" max="10" width="26.7181818181818" customWidth="1"/>
     <col min="11" max="11" width="37" customWidth="1"/>
-    <col min="12" max="12" width="36.4285714285714" customWidth="1"/>
+    <col min="12" max="12" width="36.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="90" spans="1:7">
+    <row r="2" ht="87" spans="1:7">
       <c r="A2" s="43" t="s">
         <v>467</v>
       </c>
@@ -20629,7 +20763,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" ht="60" spans="1:8">
+    <row r="4" ht="43.5" spans="1:8">
       <c r="A4" s="43" t="s">
         <v>469</v>
       </c>
@@ -20652,14 +20786,14 @@
         <v>475</v>
       </c>
     </row>
-    <row r="5" ht="15" spans="1:4">
+    <row r="5" ht="14.5" spans="1:4">
       <c r="A5" s="43"/>
       <c r="C5" s="8" t="s">
         <v>476</v>
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="7" ht="15" spans="1:7">
+    <row r="7" ht="14.5" spans="1:7">
       <c r="A7" s="43" t="s">
         <v>477</v>
       </c>
@@ -20726,18 +20860,18 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="14" ht="15" spans="1:1">
+    <row r="14" ht="14.5" spans="1:1">
       <c r="A14" s="46" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="15" ht="30" spans="1:3">
+    <row r="15" ht="29" spans="1:3">
       <c r="A15" s="46"/>
       <c r="C15" s="44" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="17" ht="90" spans="1:7">
+    <row r="17" ht="87" spans="1:7">
       <c r="A17" s="46" t="s">
         <v>493</v>
       </c>
@@ -20755,7 +20889,7 @@
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" ht="120" spans="1:6">
+    <row r="18" ht="101.5" spans="1:6">
       <c r="A18" s="46"/>
       <c r="C18" s="48" t="s">
         <v>498</v>
@@ -20770,7 +20904,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="20" ht="105" spans="1:12">
+    <row r="20" ht="101.5" spans="1:12">
       <c r="A20" s="46" t="s">
         <v>502</v>
       </c>
@@ -20805,7 +20939,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="21" ht="105" spans="1:12">
+    <row r="21" ht="101.5" spans="1:12">
       <c r="A21" s="46"/>
       <c r="C21" s="47" t="s">
         <v>513</v>
@@ -20836,7 +20970,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" ht="135" spans="1:6">
+    <row r="23" ht="130.5" spans="1:6">
       <c r="A23" s="49" t="s">
         <v>522</v>
       </c>
@@ -20858,7 +20992,7 @@
       <c r="E24" s="50"/>
       <c r="F24" s="51"/>
     </row>
-    <row r="25" ht="150" spans="1:6">
+    <row r="25" ht="145" spans="1:6">
       <c r="A25" s="46" t="s">
         <v>526</v>
       </c>
@@ -20904,7 +21038,7 @@
       <c r="E28" s="54"/>
       <c r="F28" s="51"/>
     </row>
-    <row r="30" ht="60" spans="1:8">
+    <row r="30" ht="43.5" spans="1:8">
       <c r="A30" s="46" t="s">
         <v>535</v>
       </c>
@@ -20919,7 +21053,7 @@
       <c r="G30" s="47"/>
       <c r="H30" s="48"/>
     </row>
-    <row r="31" ht="45" spans="1:8">
+    <row r="31" ht="43.5" spans="1:8">
       <c r="A31" s="46"/>
       <c r="C31" s="10"/>
       <c r="D31" s="14" t="s">
@@ -20974,7 +21108,7 @@
       <c r="G34" s="47"/>
       <c r="H34" s="48"/>
     </row>
-    <row r="35" ht="105" spans="1:9">
+    <row r="35" ht="87" spans="1:9">
       <c r="A35" s="46" t="s">
         <v>547</v>
       </c>
@@ -21000,7 +21134,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="36" ht="120" spans="1:9">
+    <row r="36" ht="116" spans="1:9">
       <c r="A36" s="46"/>
       <c r="C36" s="44" t="s">
         <v>555</v>
@@ -21060,7 +21194,7 @@
       <c r="G40" s="47"/>
       <c r="H40" s="48"/>
     </row>
-    <row r="41" ht="90" spans="1:8">
+    <row r="41" ht="87" spans="1:8">
       <c r="A41" s="46" t="s">
         <v>561</v>
       </c>
@@ -21083,7 +21217,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="42" ht="67.5" spans="1:6">
+    <row r="42" ht="64.5" spans="1:6">
       <c r="A42" s="46"/>
       <c r="C42" s="56" t="s">
         <v>568</v>
@@ -21098,7 +21232,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="43" ht="82.5" spans="1:8">
+    <row r="43" ht="77.5" spans="1:8">
       <c r="A43" s="46"/>
       <c r="C43" s="56" t="s">
         <v>572</v>
@@ -21135,7 +21269,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="46" ht="147.75" spans="1:6">
+    <row r="46" ht="145.5" spans="1:6">
       <c r="A46" s="46"/>
       <c r="C46" s="34" t="str">
         <f>_xlfn.DISPIMG("ID_4EFB6A3E5CD04B4B827C354B77123F9F",1)</f>
@@ -21180,64 +21314,64 @@
   <sheetPr/>
   <dimension ref="A2:AU135"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A92" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="B137" sqref="B137"/>
+      <selection pane="topRight" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="25.5"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="25"/>
   <cols>
-    <col min="1" max="1" width="41.6095238095238" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.0190476190476" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5047619047619" style="4" customWidth="1"/>
-    <col min="4" max="4" width="36.5714285714286" style="7" customWidth="1"/>
-    <col min="5" max="5" width="45.8380952380952" customWidth="1"/>
-    <col min="6" max="6" width="29.4380952380952" customWidth="1"/>
-    <col min="7" max="7" width="33.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="41.6090909090909" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.0181818181818" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5090909090909" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36.5727272727273" style="7" customWidth="1"/>
+    <col min="5" max="5" width="45.8363636363636" customWidth="1"/>
+    <col min="6" max="6" width="29.4363636363636" customWidth="1"/>
+    <col min="7" max="7" width="33.2818181818182" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="9" width="27.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="33.4095238095238" customWidth="1"/>
-    <col min="11" max="11" width="31.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="31.0571428571429" customWidth="1"/>
-    <col min="13" max="13" width="31.6666666666667" customWidth="1"/>
-    <col min="14" max="14" width="25.8285714285714" customWidth="1"/>
-    <col min="15" max="15" width="38.2571428571429" customWidth="1"/>
-    <col min="16" max="16" width="27.8190476190476" customWidth="1"/>
-    <col min="17" max="17" width="59.1238095238095" customWidth="1"/>
-    <col min="18" max="18" width="41.2285714285714" customWidth="1"/>
-    <col min="19" max="19" width="28.0666666666667" customWidth="1"/>
-    <col min="20" max="20" width="37.1428571428571" customWidth="1"/>
-    <col min="21" max="21" width="38.8761904761905" customWidth="1"/>
-    <col min="22" max="22" width="21.8571428571429" customWidth="1"/>
-    <col min="23" max="23" width="34.2857142857143" customWidth="1"/>
-    <col min="24" max="24" width="31.3047619047619" customWidth="1"/>
-    <col min="25" max="25" width="37.6380952380952" customWidth="1"/>
+    <col min="9" max="9" width="27.5727272727273" customWidth="1"/>
+    <col min="10" max="10" width="33.4090909090909" customWidth="1"/>
+    <col min="11" max="11" width="31.2818181818182" customWidth="1"/>
+    <col min="12" max="12" width="31.0545454545455" customWidth="1"/>
+    <col min="13" max="13" width="31.6636363636364" customWidth="1"/>
+    <col min="14" max="14" width="25.8272727272727" customWidth="1"/>
+    <col min="15" max="15" width="38.2545454545455" customWidth="1"/>
+    <col min="16" max="16" width="27.8181818181818" customWidth="1"/>
+    <col min="17" max="17" width="59.1272727272727" customWidth="1"/>
+    <col min="18" max="18" width="41.2272727272727" customWidth="1"/>
+    <col min="19" max="19" width="28.0636363636364" customWidth="1"/>
+    <col min="20" max="20" width="37.1454545454545" customWidth="1"/>
+    <col min="21" max="21" width="38.8727272727273" customWidth="1"/>
+    <col min="22" max="22" width="21.8545454545455" customWidth="1"/>
+    <col min="23" max="23" width="34.2818181818182" customWidth="1"/>
+    <col min="24" max="24" width="31.3090909090909" customWidth="1"/>
+    <col min="25" max="25" width="37.6363636363636" customWidth="1"/>
     <col min="26" max="26" width="43.6" customWidth="1"/>
-    <col min="27" max="27" width="41.9809523809524" customWidth="1"/>
-    <col min="28" max="28" width="28.4380952380952" customWidth="1"/>
-    <col min="29" max="29" width="33.7904761904762" customWidth="1"/>
-    <col min="30" max="30" width="26.4571428571429" customWidth="1"/>
-    <col min="31" max="31" width="43.7238095238095" customWidth="1"/>
-    <col min="32" max="32" width="23.2285714285714" customWidth="1"/>
-    <col min="33" max="33" width="41.2380952380952" customWidth="1"/>
-    <col min="34" max="34" width="28.9428571428571" customWidth="1"/>
-    <col min="35" max="35" width="24.7142857142857" customWidth="1"/>
-    <col min="36" max="36" width="24.5904761904762" customWidth="1"/>
+    <col min="27" max="27" width="41.9818181818182" customWidth="1"/>
+    <col min="28" max="28" width="28.4363636363636" customWidth="1"/>
+    <col min="29" max="29" width="33.7909090909091" customWidth="1"/>
+    <col min="30" max="30" width="26.4545454545455" customWidth="1"/>
+    <col min="31" max="31" width="43.7272727272727" customWidth="1"/>
+    <col min="32" max="32" width="23.2272727272727" customWidth="1"/>
+    <col min="33" max="33" width="41.2363636363636" customWidth="1"/>
+    <col min="34" max="34" width="28.9454545454545" customWidth="1"/>
+    <col min="35" max="35" width="24.7181818181818" customWidth="1"/>
+    <col min="36" max="36" width="24.5909090909091" customWidth="1"/>
     <col min="37" max="37" width="29.8" customWidth="1"/>
-    <col min="38" max="38" width="42.2285714285714" customWidth="1"/>
-    <col min="39" max="39" width="21.8571428571429" customWidth="1"/>
-    <col min="40" max="40" width="26.952380952381" customWidth="1"/>
-    <col min="41" max="41" width="26.3333333333333" customWidth="1"/>
-    <col min="42" max="42" width="24.7142857142857" customWidth="1"/>
-    <col min="43" max="43" width="26.2095238095238" customWidth="1"/>
-    <col min="44" max="44" width="24.9619047619048" customWidth="1"/>
-    <col min="45" max="45" width="25.8285714285714" customWidth="1"/>
-    <col min="46" max="46" width="20.3619047619048" customWidth="1"/>
-    <col min="47" max="47" width="21.1142857142857" customWidth="1"/>
+    <col min="38" max="38" width="42.2272727272727" customWidth="1"/>
+    <col min="39" max="39" width="21.8545454545455" customWidth="1"/>
+    <col min="40" max="40" width="26.9545454545455" customWidth="1"/>
+    <col min="41" max="41" width="26.3363636363636" customWidth="1"/>
+    <col min="42" max="42" width="24.7181818181818" customWidth="1"/>
+    <col min="43" max="43" width="26.2090909090909" customWidth="1"/>
+    <col min="44" max="44" width="24.9636363636364" customWidth="1"/>
+    <col min="45" max="45" width="25.8272727272727" customWidth="1"/>
+    <col min="46" max="46" width="20.3636363636364" customWidth="1"/>
+    <col min="47" max="47" width="21.1181818181818" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="75" spans="1:7">
+    <row r="2" ht="72.5" spans="1:7">
       <c r="A2" s="6" t="s">
         <v>583</v>
       </c>
@@ -21324,7 +21458,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="12" ht="20.25" spans="1:1">
+    <row r="12" ht="21" spans="1:1">
       <c r="A12" s="11" t="s">
         <v>597</v>
       </c>
@@ -21334,7 +21468,7 @@
       <c r="D13" s="16"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="14" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A14" s="18" t="s">
         <v>598</v>
       </c>
@@ -21366,7 +21500,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="42.75" spans="1:10">
+    <row r="15" s="1" customFormat="1" ht="42" spans="1:10">
       <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>608</v>
@@ -21396,7 +21530,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="16" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A16" s="18"/>
       <c r="B16" s="2" t="s">
         <v>617</v>
@@ -21410,7 +21544,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="17" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A17" s="18"/>
       <c r="B17" s="2" t="s">
         <v>618</v>
@@ -21424,7 +21558,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="18" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A18" s="18"/>
       <c r="C18" s="2"/>
       <c r="D18" s="21"/>
@@ -21435,7 +21569,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="19" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A19" s="18" t="s">
         <v>619</v>
       </c>
@@ -21459,7 +21593,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="57.75" spans="1:10">
+    <row r="20" s="1" customFormat="1" ht="56.5" spans="1:10">
       <c r="A20" s="18"/>
       <c r="B20" s="1" t="s">
         <v>608</v>
@@ -21481,7 +21615,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="21" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A21" s="18"/>
       <c r="B21" s="2" t="s">
         <v>617</v>
@@ -21495,7 +21629,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="22" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>618</v>
@@ -21509,7 +21643,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="23" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A23" s="18"/>
       <c r="C23" s="2"/>
       <c r="D23" s="21"/>
@@ -21520,7 +21654,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="24" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A24" s="18" t="s">
         <v>628</v>
       </c>
@@ -21558,7 +21692,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="26" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A26" s="18"/>
       <c r="B26" s="2" t="s">
         <v>617</v>
@@ -21572,7 +21706,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="27" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A27" s="18"/>
       <c r="B27" s="2" t="s">
         <v>618</v>
@@ -21586,7 +21720,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="28" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A28" s="18"/>
       <c r="C28" s="2"/>
       <c r="D28" s="21"/>
@@ -21597,7 +21731,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="29" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A29" s="18" t="s">
         <v>633</v>
       </c>
@@ -21625,7 +21759,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="45" spans="1:10">
+    <row r="30" s="1" customFormat="1" ht="43.5" spans="1:10">
       <c r="A30" s="18"/>
       <c r="B30" s="1" t="s">
         <v>608</v>
@@ -21651,7 +21785,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="31" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
         <v>617</v>
@@ -21665,7 +21799,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="32" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
         <v>618</v>
@@ -21679,7 +21813,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="33" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A33" s="18"/>
       <c r="C33" s="2"/>
       <c r="D33" s="21"/>
@@ -21690,7 +21824,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="34" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A34" s="18" t="s">
         <v>646</v>
       </c>
@@ -21736,7 +21870,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="36" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A36" s="18"/>
       <c r="B36" s="2" t="s">
         <v>617</v>
@@ -21750,7 +21884,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="37" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A37" s="18"/>
       <c r="B37" s="2" t="s">
         <v>618</v>
@@ -21764,7 +21898,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="38" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A38" s="18"/>
       <c r="C38" s="2"/>
       <c r="D38" s="21"/>
@@ -21775,7 +21909,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="39" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A39" s="18" t="s">
         <v>655</v>
       </c>
@@ -21797,7 +21931,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" s="1" customFormat="1" ht="45" spans="1:10">
+    <row r="40" s="1" customFormat="1" ht="43.5" spans="1:10">
       <c r="A40" s="18"/>
       <c r="B40" s="1" t="s">
         <v>608</v>
@@ -21817,7 +21951,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="41" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A41" s="18"/>
       <c r="B41" s="2" t="s">
         <v>617</v>
@@ -21831,7 +21965,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="42" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A42" s="18"/>
       <c r="B42" s="2" t="s">
         <v>618</v>
@@ -21845,7 +21979,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="43" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A43" s="18"/>
       <c r="C43" s="2"/>
       <c r="D43" s="21"/>
@@ -21856,7 +21990,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="44" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A44" s="18" t="s">
         <v>662</v>
       </c>
@@ -21880,7 +22014,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="39" spans="1:10">
+    <row r="45" s="1" customFormat="1" ht="38" spans="1:10">
       <c r="A45" s="18"/>
       <c r="B45" s="1" t="s">
         <v>608</v>
@@ -21902,7 +22036,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="46" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A46" s="18"/>
       <c r="B46" s="2" t="s">
         <v>617</v>
@@ -21916,7 +22050,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="15" spans="1:10">
+    <row r="47" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A47" s="18"/>
       <c r="B47" s="2" t="s">
         <v>618</v>
@@ -21930,7 +22064,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" s="1" customFormat="1" ht="20.25" spans="1:10">
+    <row r="48" s="1" customFormat="1" ht="21" spans="1:10">
       <c r="A48" s="18"/>
       <c r="C48" s="2"/>
       <c r="D48" s="21"/>
@@ -21941,7 +22075,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" s="2" customFormat="1" ht="15" spans="1:6">
+    <row r="49" s="2" customFormat="1" ht="14.5" spans="1:6">
       <c r="A49" s="31" t="s">
         <v>671</v>
       </c>
@@ -21961,7 +22095,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="50" s="2" customFormat="1" ht="45" spans="1:6">
+    <row r="50" s="2" customFormat="1" ht="43.5" spans="1:6">
       <c r="A50" s="31"/>
       <c r="B50" s="2" t="s">
         <v>608</v>
@@ -21979,25 +22113,25 @@
         <v>678</v>
       </c>
     </row>
-    <row r="51" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="51" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A51" s="31"/>
       <c r="B51" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D51" s="21"/>
     </row>
-    <row r="52" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="52" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A52" s="31"/>
       <c r="B52" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D52" s="21"/>
     </row>
-    <row r="53" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="53" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A53" s="31"/>
       <c r="D53" s="21"/>
     </row>
-    <row r="54" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="54" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A54" s="31" t="s">
         <v>679</v>
       </c>
@@ -22011,7 +22145,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="55" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="55" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A55" s="31"/>
       <c r="B55" s="2" t="s">
         <v>608</v>
@@ -22023,25 +22157,25 @@
         <v>683</v>
       </c>
     </row>
-    <row r="56" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="56" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A56" s="31"/>
       <c r="B56" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D56" s="21"/>
     </row>
-    <row r="57" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="57" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A57" s="31"/>
       <c r="B57" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D57" s="21"/>
     </row>
-    <row r="58" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="58" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A58" s="31"/>
       <c r="D58" s="21"/>
     </row>
-    <row r="59" s="2" customFormat="1" ht="15" spans="1:11">
+    <row r="59" s="2" customFormat="1" ht="14.5" spans="1:11">
       <c r="A59" s="31" t="s">
         <v>684</v>
       </c>
@@ -22076,7 +22210,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="60" s="2" customFormat="1" ht="51" spans="1:11">
+    <row r="60" s="2" customFormat="1" ht="50" spans="1:11">
       <c r="A60" s="31"/>
       <c r="B60" s="2" t="s">
         <v>608</v>
@@ -22109,25 +22243,25 @@
         <v>702</v>
       </c>
     </row>
-    <row r="61" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="61" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A61" s="31"/>
       <c r="B61" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D61" s="21"/>
     </row>
-    <row r="62" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="62" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A62" s="31"/>
       <c r="B62" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D62" s="21"/>
     </row>
-    <row r="63" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="63" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A63" s="31"/>
       <c r="D63" s="21"/>
     </row>
-    <row r="64" s="2" customFormat="1" ht="15" spans="1:10">
+    <row r="64" s="2" customFormat="1" ht="14.5" spans="1:10">
       <c r="A64" s="31" t="s">
         <v>703</v>
       </c>
@@ -22159,7 +22293,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="65" s="2" customFormat="1" ht="45" spans="1:10">
+    <row r="65" s="2" customFormat="1" ht="43.5" spans="1:10">
       <c r="A65" s="31"/>
       <c r="B65" s="2" t="s">
         <v>608</v>
@@ -22189,25 +22323,25 @@
         <v>718</v>
       </c>
     </row>
-    <row r="66" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="66" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A66" s="31"/>
       <c r="B66" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D66" s="21"/>
     </row>
-    <row r="67" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="67" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A67" s="31"/>
       <c r="B67" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D67" s="21"/>
     </row>
-    <row r="68" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="68" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A68" s="31"/>
       <c r="D68" s="21"/>
     </row>
-    <row r="69" s="2" customFormat="1" ht="15" spans="1:6">
+    <row r="69" s="2" customFormat="1" ht="14.5" spans="1:6">
       <c r="A69" s="31" t="s">
         <v>719</v>
       </c>
@@ -22227,7 +22361,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="70" s="2" customFormat="1" ht="45" spans="1:6">
+    <row r="70" s="2" customFormat="1" ht="43.5" spans="1:6">
       <c r="A70" s="31"/>
       <c r="B70" s="2" t="s">
         <v>608</v>
@@ -22245,25 +22379,25 @@
         <v>726</v>
       </c>
     </row>
-    <row r="71" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="71" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A71" s="31"/>
       <c r="B71" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D71" s="21"/>
     </row>
-    <row r="72" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="72" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A72" s="31"/>
       <c r="B72" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D72" s="21"/>
     </row>
-    <row r="73" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="73" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A73" s="31"/>
       <c r="D73" s="21"/>
     </row>
-    <row r="74" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="74" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A74" s="31" t="s">
         <v>727</v>
       </c>
@@ -22275,7 +22409,7 @@
       </c>
       <c r="D74" s="21"/>
     </row>
-    <row r="75" s="2" customFormat="1" ht="30" spans="1:4">
+    <row r="75" s="2" customFormat="1" ht="28.5" spans="1:4">
       <c r="A75" s="31"/>
       <c r="B75" s="2" t="s">
         <v>608</v>
@@ -22285,25 +22419,25 @@
       </c>
       <c r="D75" s="21"/>
     </row>
-    <row r="76" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="76" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A76" s="31"/>
       <c r="B76" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D76" s="21"/>
     </row>
-    <row r="77" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="77" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A77" s="31"/>
       <c r="B77" s="2" t="s">
         <v>618</v>
       </c>
       <c r="D77" s="21"/>
     </row>
-    <row r="78" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="78" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A78" s="31"/>
       <c r="D78" s="21"/>
     </row>
-    <row r="79" s="2" customFormat="1" ht="15" spans="1:38">
+    <row r="79" s="2" customFormat="1" ht="14.5" spans="1:38">
       <c r="A79" s="31" t="s">
         <v>730</v>
       </c>
@@ -22419,7 +22553,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="80" s="2" customFormat="1" ht="135" spans="1:38">
+    <row r="80" s="2" customFormat="1" ht="130.5" spans="1:38">
       <c r="A80" s="31"/>
       <c r="B80" s="2" t="s">
         <v>608</v>
@@ -22533,14 +22667,14 @@
         <v>799</v>
       </c>
     </row>
-    <row r="81" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="81" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A81" s="31"/>
       <c r="B81" s="2" t="s">
         <v>617</v>
       </c>
       <c r="D81" s="21"/>
     </row>
-    <row r="82" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="82" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A82" s="31"/>
       <c r="B82" s="2" t="s">
         <v>618</v>
@@ -22548,12 +22682,12 @@
       <c r="C82" s="35"/>
       <c r="D82" s="35"/>
     </row>
-    <row r="83" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="83" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A83" s="31"/>
       <c r="C83" s="35"/>
       <c r="D83" s="36"/>
     </row>
-    <row r="84" s="2" customFormat="1" ht="15" spans="1:6">
+    <row r="84" s="2" customFormat="1" ht="14.5" spans="1:6">
       <c r="A84" s="31" t="s">
         <v>800</v>
       </c>
@@ -22573,7 +22707,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="85" s="3" customFormat="1" ht="60" spans="1:6">
+    <row r="85" s="3" customFormat="1" ht="58" spans="1:6">
       <c r="A85" s="31"/>
       <c r="B85" s="3" t="s">
         <v>608</v>
@@ -22591,7 +22725,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="86" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="86" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A86" s="31"/>
       <c r="B86" s="2" t="s">
         <v>617</v>
@@ -22599,7 +22733,7 @@
       <c r="C86" s="35"/>
       <c r="D86" s="36"/>
     </row>
-    <row r="87" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="87" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A87" s="31"/>
       <c r="B87" s="2" t="s">
         <v>618</v>
@@ -22607,12 +22741,12 @@
       <c r="C87" s="35"/>
       <c r="D87" s="36"/>
     </row>
-    <row r="88" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="88" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A88" s="31"/>
       <c r="C88" s="35"/>
       <c r="D88" s="36"/>
     </row>
-    <row r="89" s="2" customFormat="1" ht="15" spans="1:18">
+    <row r="89" s="2" customFormat="1" ht="14.5" spans="1:18">
       <c r="A89" s="31" t="s">
         <v>806</v>
       </c>
@@ -22668,7 +22802,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="90" s="3" customFormat="1" ht="105" spans="1:18">
+    <row r="90" s="3" customFormat="1" ht="101.5" spans="1:18">
       <c r="A90" s="31"/>
       <c r="B90" s="3" t="s">
         <v>608</v>
@@ -22722,7 +22856,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="91" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="91" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A91" s="31"/>
       <c r="B91" s="2" t="s">
         <v>617</v>
@@ -22730,7 +22864,7 @@
       <c r="C91" s="35"/>
       <c r="D91" s="36"/>
     </row>
-    <row r="92" s="2" customFormat="1" ht="15" spans="1:4">
+    <row r="92" s="2" customFormat="1" ht="14.5" spans="1:4">
       <c r="A92" s="31"/>
       <c r="B92" s="2" t="s">
         <v>618</v>
@@ -22738,12 +22872,12 @@
       <c r="C92" s="35"/>
       <c r="D92" s="36"/>
     </row>
-    <row r="93" s="2" customFormat="1" ht="20.25" spans="1:4">
+    <row r="93" s="2" customFormat="1" ht="21" spans="1:4">
       <c r="A93" s="31"/>
       <c r="C93" s="35"/>
       <c r="D93" s="36"/>
     </row>
-    <row r="94" s="2" customFormat="1" ht="15" spans="1:24">
+    <row r="94" s="2" customFormat="1" ht="14.5" spans="1:24">
       <c r="A94" s="31" t="s">
         <v>839</v>
       </c>
@@ -22817,7 +22951,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="95" s="2" customFormat="1" ht="75" spans="1:24">
+    <row r="95" s="2" customFormat="1" ht="72" customHeight="1" spans="1:24">
       <c r="A95" s="31"/>
       <c r="B95" s="3" t="s">
         <v>608</v>
@@ -22889,7 +23023,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="96" ht="15" spans="1:4">
+    <row r="96" ht="14.5" spans="1:4">
       <c r="A96" s="31"/>
       <c r="B96" s="2" t="s">
         <v>617</v>
@@ -22897,7 +23031,7 @@
       <c r="C96" s="35"/>
       <c r="D96" s="35"/>
     </row>
-    <row r="97" ht="15" spans="1:4">
+    <row r="97" ht="14.5" spans="1:4">
       <c r="A97" s="31"/>
       <c r="B97" s="2" t="s">
         <v>618</v>
@@ -22909,7 +23043,7 @@
       <c r="C98" s="35"/>
       <c r="D98" s="36"/>
     </row>
-    <row r="99" ht="15" spans="1:5">
+    <row r="99" ht="14.5" spans="1:5">
       <c r="A99" s="31" t="s">
         <v>881</v>
       </c>
@@ -22926,7 +23060,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="100" ht="45" spans="1:5">
+    <row r="100" ht="43.5" spans="1:5">
       <c r="A100" s="31"/>
       <c r="B100" s="3" t="s">
         <v>608</v>
@@ -22941,7 +23075,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="101" ht="15" spans="1:4">
+    <row r="101" ht="14.5" spans="1:4">
       <c r="A101" s="31"/>
       <c r="B101" s="2" t="s">
         <v>617</v>
@@ -22949,7 +23083,7 @@
       <c r="C101" s="35"/>
       <c r="D101" s="36"/>
     </row>
-    <row r="102" ht="15" spans="1:4">
+    <row r="102" ht="14.5" spans="1:4">
       <c r="A102" s="31"/>
       <c r="B102" s="2" t="s">
         <v>618</v>
@@ -22961,7 +23095,7 @@
       <c r="C103" s="35"/>
       <c r="D103" s="36"/>
     </row>
-    <row r="104" ht="15" spans="1:9">
+    <row r="104" ht="14.5" spans="1:9">
       <c r="A104" s="31" t="s">
         <v>885</v>
       </c>
@@ -22990,7 +23124,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="105" ht="60" spans="1:9">
+    <row r="105" ht="43.5" spans="1:9">
       <c r="A105" s="31"/>
       <c r="B105" s="3" t="s">
         <v>608</v>
@@ -23017,7 +23151,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="106" ht="15" spans="1:4">
+    <row r="106" ht="14.5" spans="1:4">
       <c r="A106" s="31"/>
       <c r="B106" s="2" t="s">
         <v>617</v>
@@ -23025,7 +23159,7 @@
       <c r="C106" s="35"/>
       <c r="D106" s="35"/>
     </row>
-    <row r="107" ht="15" spans="1:4">
+    <row r="107" ht="14.5" spans="1:4">
       <c r="A107" s="31"/>
       <c r="B107" s="2" t="s">
         <v>618</v>
@@ -23037,7 +23171,7 @@
       <c r="C108" s="35"/>
       <c r="D108" s="36"/>
     </row>
-    <row r="109" ht="15" spans="1:5">
+    <row r="109" ht="14.5" spans="1:5">
       <c r="A109" s="31" t="s">
         <v>894</v>
       </c>
@@ -23054,7 +23188,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="110" ht="120" spans="1:5">
+    <row r="110" ht="116" spans="1:5">
       <c r="A110" s="31"/>
       <c r="B110" s="3" t="s">
         <v>608</v>
@@ -23069,7 +23203,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="111" ht="15" spans="1:4">
+    <row r="111" ht="14.5" spans="1:4">
       <c r="A111" s="31"/>
       <c r="B111" s="2" t="s">
         <v>617</v>
@@ -23077,7 +23211,7 @@
       <c r="C111" s="35"/>
       <c r="D111" s="36"/>
     </row>
-    <row r="112" ht="15" spans="1:4">
+    <row r="112" ht="14.5" spans="1:4">
       <c r="A112" s="31"/>
       <c r="B112" s="2" t="s">
         <v>618</v>
@@ -23089,7 +23223,7 @@
       <c r="C113" s="35"/>
       <c r="D113" s="36"/>
     </row>
-    <row r="114" ht="15" spans="1:4">
+    <row r="114" ht="14.5" spans="1:4">
       <c r="A114" s="31" t="s">
         <v>901</v>
       </c>
@@ -23103,7 +23237,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="115" ht="15" spans="1:4">
+    <row r="115" ht="14.5" spans="1:4">
       <c r="A115" s="31"/>
       <c r="B115" s="3" t="s">
         <v>608</v>
@@ -23115,7 +23249,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="116" ht="15" spans="1:4">
+    <row r="116" ht="14.5" spans="1:4">
       <c r="A116" s="31"/>
       <c r="B116" s="2" t="s">
         <v>617</v>
@@ -23123,7 +23257,7 @@
       <c r="C116" s="35"/>
       <c r="D116" s="36"/>
     </row>
-    <row r="117" ht="15" spans="1:4">
+    <row r="117" ht="14.5" spans="1:4">
       <c r="A117" s="31"/>
       <c r="B117" s="2" t="s">
         <v>618</v>
@@ -23135,7 +23269,7 @@
       <c r="C118" s="35"/>
       <c r="D118" s="35"/>
     </row>
-    <row r="119" ht="15" spans="1:4">
+    <row r="119" ht="14.5" spans="1:4">
       <c r="A119" s="31" t="s">
         <v>906</v>
       </c>
@@ -23145,7 +23279,7 @@
       <c r="C119" s="35"/>
       <c r="D119" s="36"/>
     </row>
-    <row r="120" ht="15" spans="1:4">
+    <row r="120" ht="14.5" spans="1:4">
       <c r="A120" s="31"/>
       <c r="B120" s="3" t="s">
         <v>608</v>
@@ -23153,7 +23287,7 @@
       <c r="C120" s="35"/>
       <c r="D120" s="36"/>
     </row>
-    <row r="121" ht="15" spans="1:4">
+    <row r="121" ht="14.5" spans="1:4">
       <c r="A121" s="31"/>
       <c r="B121" s="2" t="s">
         <v>617</v>
@@ -23161,7 +23295,7 @@
       <c r="C121" s="35"/>
       <c r="D121" s="36"/>
     </row>
-    <row r="122" ht="15" spans="1:4">
+    <row r="122" ht="14.5" spans="1:4">
       <c r="A122" s="31"/>
       <c r="B122" s="2" t="s">
         <v>618</v>
@@ -23181,7 +23315,7 @@
       <c r="C125" s="35"/>
       <c r="D125" s="36"/>
     </row>
-    <row r="128" s="4" customFormat="1" ht="30" spans="1:47">
+    <row r="128" s="4" customFormat="1" ht="14.5" spans="1:47">
       <c r="A128" s="38" t="s">
         <v>907</v>
       </c>
@@ -23465,7 +23599,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="131" s="1" customFormat="1" ht="15" spans="1:35">
+    <row r="131" s="1" customFormat="1" ht="14.5" spans="1:35">
       <c r="A131" s="38" t="s">
         <v>1000</v>
       </c>
@@ -23572,7 +23706,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="132" s="4" customFormat="1" ht="75" spans="1:35">
+    <row r="132" s="4" customFormat="1" ht="72.5" spans="1:35">
       <c r="A132" s="38"/>
       <c r="B132" s="34" t="s">
         <v>954</v>
@@ -23677,7 +23811,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="134" ht="15" spans="1:43">
+    <row r="134" ht="14.5" spans="1:43">
       <c r="A134" s="38" t="s">
         <v>1067</v>
       </c>
@@ -23808,7 +23942,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="135" s="5" customFormat="1" ht="90" spans="1:43">
+    <row r="135" s="5" customFormat="1" ht="87" spans="1:43">
       <c r="A135" s="38"/>
       <c r="B135" s="34" t="s">
         <v>954</v>
@@ -23987,18 +24121,18 @@
       <selection pane="topRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="21" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="22.8571428571429" style="43" customWidth="1"/>
-    <col min="3" max="3" width="38.7142857142857" style="4" customWidth="1"/>
-    <col min="4" max="4" width="43.2857142857143" style="4" customWidth="1"/>
-    <col min="5" max="5" width="43.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="68.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="36.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="36.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="22.8545454545455" style="43" customWidth="1"/>
+    <col min="3" max="3" width="38.7181818181818" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.2818181818182" style="4" customWidth="1"/>
+    <col min="5" max="5" width="43.2818181818182" customWidth="1"/>
+    <col min="6" max="6" width="68.7181818181818" customWidth="1"/>
+    <col min="7" max="7" width="36.2818181818182" customWidth="1"/>
+    <col min="8" max="8" width="36.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="105" spans="1:8">
+    <row r="2" ht="101.5" spans="1:8">
       <c r="A2" s="43" t="s">
         <v>130</v>
       </c>
@@ -24036,7 +24170,7 @@
       <selection activeCell="J55" sqref="J55:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -24054,31 +24188,31 @@
       <selection pane="topRight" activeCell="J55" sqref="J55:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.7142857142857" style="8" customWidth="1"/>
-    <col min="2" max="2" width="55.4285714285714" style="8" customWidth="1"/>
-    <col min="3" max="3" width="45.5714285714286" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.1428571428571" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7142857142857" style="4" customWidth="1"/>
-    <col min="6" max="6" width="49.7142857142857" style="4" customWidth="1"/>
-    <col min="7" max="7" width="39.4285714285714" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.7181818181818" style="8" customWidth="1"/>
+    <col min="2" max="2" width="55.4272727272727" style="8" customWidth="1"/>
+    <col min="3" max="3" width="45.5727272727273" style="4" customWidth="1"/>
+    <col min="4" max="4" width="42.1454545454545" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7181818181818" style="4" customWidth="1"/>
+    <col min="6" max="6" width="49.7181818181818" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.4272727272727" style="4" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
-    <col min="9" max="9" width="49.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="49.2818181818182" customWidth="1"/>
     <col min="10" max="10" width="49" customWidth="1"/>
-    <col min="11" max="11" width="42.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="42.5727272727273" customWidth="1"/>
     <col min="12" max="12" width="32" customWidth="1"/>
-    <col min="13" max="13" width="33.2857142857143" customWidth="1"/>
-    <col min="14" max="14" width="38.7142857142857" customWidth="1"/>
-    <col min="15" max="15" width="25.7142857142857" customWidth="1"/>
+    <col min="13" max="13" width="33.2818181818182" customWidth="1"/>
+    <col min="14" max="14" width="38.7181818181818" customWidth="1"/>
+    <col min="15" max="15" width="25.7181818181818" customWidth="1"/>
     <col min="16" max="16" width="47" customWidth="1"/>
-    <col min="17" max="17" width="26.2857142857143" customWidth="1"/>
+    <col min="17" max="17" width="26.2818181818182" customWidth="1"/>
     <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="20.7142857142857" customWidth="1"/>
-    <col min="20" max="20" width="17.1428571428571" customWidth="1"/>
+    <col min="19" max="19" width="20.7181818181818" customWidth="1"/>
+    <col min="20" max="20" width="17.1454545454545" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="95" customFormat="1" ht="23.25" spans="1:20">
+    <row r="1" s="95" customFormat="1" ht="23.5" spans="1:20">
       <c r="A1" s="96" t="s">
         <v>137</v>
       </c>
@@ -24140,7 +24274,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" ht="75" spans="1:8">
+    <row r="2" ht="72.5" spans="1:8">
       <c r="A2" s="99" t="s">
         <v>140</v>
       </c>
@@ -24161,7 +24295,7 @@
       </c>
       <c r="H2" s="102"/>
     </row>
-    <row r="3" ht="20.25" spans="1:8">
+    <row r="3" ht="21" spans="1:8">
       <c r="A3" s="99"/>
       <c r="B3" s="99"/>
       <c r="C3" s="101"/>
@@ -24170,7 +24304,7 @@
       <c r="G3" s="101"/>
       <c r="H3" s="103"/>
     </row>
-    <row r="4" ht="105" spans="1:15">
+    <row r="4" ht="101.5" spans="1:15">
       <c r="A4" s="104" t="s">
         <v>146</v>
       </c>
@@ -24222,7 +24356,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" ht="90" spans="1:6">
+    <row r="6" ht="87" spans="1:6">
       <c r="A6" s="104" t="s">
         <v>162</v>
       </c>
@@ -24240,7 +24374,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" ht="150" spans="1:20">
+    <row r="8" ht="145" spans="1:20">
       <c r="A8" s="104" t="s">
         <v>167</v>
       </c>
@@ -24294,7 +24428,7 @@
       </c>
       <c r="T8" s="102"/>
     </row>
-    <row r="10" ht="75" spans="1:13">
+    <row r="10" ht="58" spans="1:13">
       <c r="A10" s="104" t="s">
         <v>183</v>
       </c>
@@ -24357,25 +24491,25 @@
       <selection activeCell="A36" sqref="A36:A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="23.4285714285714" style="63" customWidth="1"/>
-    <col min="3" max="3" width="32.8571428571429" style="64" customWidth="1"/>
-    <col min="4" max="4" width="13.4285714285714" style="65" customWidth="1"/>
-    <col min="5" max="5" width="29.4285714285714" style="66" customWidth="1"/>
-    <col min="6" max="6" width="21.2857142857143" style="65" customWidth="1"/>
-    <col min="7" max="7" width="38.5714285714286" style="66" customWidth="1"/>
-    <col min="8" max="8" width="17.2857142857143" customWidth="1"/>
-    <col min="9" max="9" width="38.8571428571429" customWidth="1"/>
-    <col min="10" max="10" width="21.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="41.4285714285714" customWidth="1"/>
-    <col min="12" max="12" width="13.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="28.8545454545455" customWidth="1"/>
+    <col min="2" max="2" width="23.4272727272727" style="63" customWidth="1"/>
+    <col min="3" max="3" width="32.8545454545455" style="64" customWidth="1"/>
+    <col min="4" max="4" width="13.4272727272727" style="65" customWidth="1"/>
+    <col min="5" max="5" width="29.4272727272727" style="66" customWidth="1"/>
+    <col min="6" max="6" width="21.2818181818182" style="65" customWidth="1"/>
+    <col min="7" max="7" width="38.5727272727273" style="66" customWidth="1"/>
+    <col min="8" max="8" width="17.2818181818182" customWidth="1"/>
+    <col min="9" max="9" width="38.8545454545455" customWidth="1"/>
+    <col min="10" max="10" width="21.2818181818182" customWidth="1"/>
+    <col min="11" max="11" width="41.4272727272727" customWidth="1"/>
+    <col min="12" max="12" width="13.4272727272727" customWidth="1"/>
     <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="14" width="13.4285714285714" customWidth="1"/>
-    <col min="15" max="15" width="33.8571428571429" customWidth="1"/>
-    <col min="16" max="16" width="19.8571428571429" customWidth="1"/>
-    <col min="17" max="17" width="32.2857142857143" customWidth="1"/>
+    <col min="14" max="14" width="13.4272727272727" customWidth="1"/>
+    <col min="15" max="15" width="33.8545454545455" customWidth="1"/>
+    <col min="16" max="16" width="19.8545454545455" customWidth="1"/>
+    <col min="17" max="17" width="32.2818181818182" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="17" spans="1:15">
@@ -24425,7 +24559,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" ht="30" spans="1:15">
+    <row r="18" ht="29" spans="1:15">
       <c r="A18" s="67"/>
       <c r="B18" s="68"/>
       <c r="C18" s="73"/>
@@ -24466,7 +24600,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" ht="30" spans="1:15">
+    <row r="19" ht="29" spans="1:15">
       <c r="A19" s="67"/>
       <c r="B19" s="68"/>
       <c r="C19" s="73"/>
@@ -24719,7 +24853,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="26" ht="30" spans="1:15">
+    <row r="26" ht="29" spans="1:15">
       <c r="A26" s="67"/>
       <c r="B26" s="68"/>
       <c r="C26" s="73"/>
@@ -24760,7 +24894,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="27" ht="30" spans="1:15">
+    <row r="27" ht="29" spans="1:15">
       <c r="A27" s="67"/>
       <c r="B27" s="68"/>
       <c r="C27" s="73"/>
@@ -25106,11 +25240,11 @@
         <v>398</v>
       </c>
     </row>
-    <row r="38" ht="31.5" spans="1:2">
+    <row r="38" ht="31" spans="1:2">
       <c r="A38" s="8"/>
       <c r="B38" s="91"/>
     </row>
-    <row r="39" ht="37.5" spans="1:9">
+    <row r="39" ht="35" spans="1:9">
       <c r="A39" s="8"/>
       <c r="B39" s="92" t="s">
         <v>399</v>
@@ -25137,11 +25271,11 @@
         <v>406</v>
       </c>
     </row>
-    <row r="40" ht="31.5" spans="1:2">
+    <row r="40" ht="31" spans="1:2">
       <c r="A40" s="8"/>
       <c r="B40" s="91"/>
     </row>
-    <row r="41" ht="31.5" spans="1:11">
+    <row r="41" ht="31" spans="1:11">
       <c r="A41" s="8"/>
       <c r="B41" s="68" t="s">
         <v>407</v>
@@ -25174,11 +25308,11 @@
         <v>416</v>
       </c>
     </row>
-    <row r="42" ht="31.5" spans="1:2">
+    <row r="42" ht="31" spans="1:2">
       <c r="A42" s="8"/>
       <c r="B42" s="68"/>
     </row>
-    <row r="43" ht="31.5" spans="1:7">
+    <row r="43" ht="31" spans="1:7">
       <c r="A43" s="8"/>
       <c r="B43" s="68" t="s">
         <v>417</v>
@@ -25199,11 +25333,11 @@
         <v>422</v>
       </c>
     </row>
-    <row r="44" ht="31.5" spans="1:2">
+    <row r="44" ht="31" spans="1:2">
       <c r="A44" s="8"/>
       <c r="B44" s="91"/>
     </row>
-    <row r="45" ht="31.5" spans="1:7">
+    <row r="45" ht="31" spans="1:7">
       <c r="A45" s="8"/>
       <c r="B45" s="68" t="s">
         <v>423</v>
@@ -25224,7 +25358,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47" ht="45" spans="3:7">
+    <row r="47" ht="43.5" spans="3:7">
       <c r="C47" s="57" t="s">
         <v>429</v>
       </c>
@@ -25270,19 +25404,19 @@
       <selection pane="topRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="18.2857142857143" style="60" customWidth="1"/>
-    <col min="2" max="2" width="48.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="49.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="47.7142857142857" customWidth="1"/>
-    <col min="5" max="5" width="61.5714285714286" customWidth="1"/>
-    <col min="6" max="6" width="45.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="45.1428571428571" customWidth="1"/>
-    <col min="8" max="8" width="41.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="18.2818181818182" style="60" customWidth="1"/>
+    <col min="2" max="2" width="48.2818181818182" customWidth="1"/>
+    <col min="3" max="3" width="49.2818181818182" customWidth="1"/>
+    <col min="4" max="4" width="47.7181818181818" customWidth="1"/>
+    <col min="5" max="5" width="61.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="45.4272727272727" customWidth="1"/>
+    <col min="7" max="7" width="45.1454545454545" customWidth="1"/>
+    <col min="8" max="8" width="41.8545454545455" customWidth="1"/>
     <col min="9" max="9" width="93" customWidth="1"/>
-    <col min="10" max="10" width="36.5714285714286" customWidth="1"/>
-    <col min="11" max="11" width="12.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="36.5727272727273" customWidth="1"/>
+    <col min="11" max="11" width="12.4272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="26" ht="63" spans="1:4">
@@ -25299,7 +25433,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" ht="165" spans="1:9">
+    <row r="28" ht="159.5" spans="1:9">
       <c r="A28" s="60" t="s">
         <v>435</v>
       </c>
@@ -25322,7 +25456,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="31" ht="255" spans="1:6">
+    <row r="31" ht="232" spans="1:6">
       <c r="A31" s="60" t="s">
         <v>442</v>
       </c>
@@ -25340,7 +25474,7 @@
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
     </row>
-    <row r="33" ht="300" spans="1:9">
+    <row r="33" ht="261" spans="1:9">
       <c r="A33" s="60" t="s">
         <v>445</v>
       </c>
@@ -25366,7 +25500,7 @@
     <row r="34" spans="2:2">
       <c r="B34" s="48"/>
     </row>
-    <row r="51" ht="90" spans="1:6">
+    <row r="51" ht="87" spans="1:6">
       <c r="A51" s="60" t="s">
         <v>451</v>
       </c>
@@ -25386,7 +25520,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="53" ht="135" spans="1:13">
+    <row r="53" ht="130.5" spans="1:13">
       <c r="A53" s="60" t="s">
         <v>457</v>
       </c>
@@ -25439,7 +25573,7 @@
       <selection activeCell="J55" sqref="J55:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -25455,7 +25589,7 @@
       <selection activeCell="J55" sqref="J55:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -25471,7 +25605,7 @@
       <selection activeCell="J55" sqref="J55:M55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>